<commit_message>
Commit of Content/Live use cases/NHS 111 Discovery frailty flagging.htm,Content/Resources/frailty codes.xlsx
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9061F031-9E78-42CD-8CE6-31B7521FBA98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6D4B09-0809-4183-9915-C22BAFA5485D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
@@ -727,7 +727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01E6FF3D-551A-4CCC-B3BF-B7EE1858AE68}" type="CELLRANGE">
+                    <a:fld id="{64CB1F2E-7D03-4179-9A48-4A8CD2315C86}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -761,7 +761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F1E2CEC-E661-4DC3-8CB9-C589160BCD25}" type="CELLRANGE">
+                    <a:fld id="{7F72C07F-DB1B-4D81-979D-62C8D32ED574}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -795,7 +795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97A3A09B-0B40-4B0F-B146-C64DDD148F5C}" type="CELLRANGE">
+                    <a:fld id="{AECCA031-A487-4DDC-9013-5E18EDEFFC4D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -829,7 +829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12ECD454-97E3-452C-9717-49E5FB9A13E7}" type="CELLRANGE">
+                    <a:fld id="{869992E5-083D-437F-80E9-4117A6C15131}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -863,7 +863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08D0EF6B-29BA-4C10-957A-DB452C186120}" type="CELLRANGE">
+                    <a:fld id="{D77AA17F-BB4E-44A0-A964-E7CC7ED6818A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -897,7 +897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B361398-F2C4-4814-9ED1-F28732B13EC6}" type="CELLRANGE">
+                    <a:fld id="{88E98155-0F5C-44B0-A0F1-E2B2CDF19F41}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -931,7 +931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77BC1E41-CD81-4A1F-ACB0-EC812FCF1BFE}" type="CELLRANGE">
+                    <a:fld id="{8A002998-59C3-484B-844B-7DDA8F13E7CD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -965,7 +965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C62242A-DF8C-4415-A2EB-771CDFC54061}" type="CELLRANGE">
+                    <a:fld id="{FD0BD1AA-3384-42CF-809A-7720C6893769}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -999,7 +999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{126176CC-34B4-4FE8-83EF-2B78B4B70A75}" type="CELLRANGE">
+                    <a:fld id="{4CAAEB60-DCC8-416E-A49D-137DA6A89BA7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1033,7 +1033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3030628D-3A40-4644-99DC-CA668E48D7E5}" type="CELLRANGE">
+                    <a:fld id="{8CB77162-68E2-4E3E-A1E2-D5A92D10E4AE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1067,7 +1067,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6160468B-718A-42D4-95CE-BEC420D417D3}" type="CELLRANGE">
+                    <a:fld id="{5FB59897-748D-4437-A4E9-A6871B70A3DF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1101,7 +1101,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACB3EDE9-284D-4CBE-8685-9F46B7F8A61E}" type="CELLRANGE">
+                    <a:fld id="{A513DD1C-BE6E-44D2-BD4D-0CCB01D34B6B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1597,7 +1597,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Totals!$A$2:$A$13</c15:sqref>
@@ -2177,7 +2177,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit of Content/Live use cases/NHS 111 Discovery frailty flagging.htm,Content/Partners/Partners.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png,Content/Resources/Images/Logos/F50.jpg,Content/Use cases.htm
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6D4B09-0809-4183-9915-C22BAFA5485D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7560DF5-B029-48FC-B8C7-04DDC627C333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
     <sheet name="Totals" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -727,7 +726,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64CB1F2E-7D03-4179-9A48-4A8CD2315C86}" type="CELLRANGE">
+                    <a:fld id="{B126A783-ABB5-4483-A304-7483DE945F42}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -761,7 +760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F72C07F-DB1B-4D81-979D-62C8D32ED574}" type="CELLRANGE">
+                    <a:fld id="{E14207AF-8DD4-4B73-A5B6-0B2A4B18414D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -795,7 +794,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AECCA031-A487-4DDC-9013-5E18EDEFFC4D}" type="CELLRANGE">
+                    <a:fld id="{5723B643-A9CC-478C-9EC0-DA2C1172391A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -829,7 +828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{869992E5-083D-437F-80E9-4117A6C15131}" type="CELLRANGE">
+                    <a:fld id="{39E6D374-7606-4B4A-81EE-175B964CD421}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -863,7 +862,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D77AA17F-BB4E-44A0-A964-E7CC7ED6818A}" type="CELLRANGE">
+                    <a:fld id="{731BE0BC-72D9-41B9-81EA-AD77CC6D4704}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -897,7 +896,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88E98155-0F5C-44B0-A0F1-E2B2CDF19F41}" type="CELLRANGE">
+                    <a:fld id="{761484A0-502E-4A79-ACE3-E320A5BE8006}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -931,7 +930,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A002998-59C3-484B-844B-7DDA8F13E7CD}" type="CELLRANGE">
+                    <a:fld id="{1C78CF31-42FA-4658-A952-EE65697BFF53}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -965,7 +964,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD0BD1AA-3384-42CF-809A-7720C6893769}" type="CELLRANGE">
+                    <a:fld id="{C34B9966-3200-42B6-8BA0-1F7483D2AF93}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -999,7 +998,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CAAEB60-DCC8-416E-A49D-137DA6A89BA7}" type="CELLRANGE">
+                    <a:fld id="{0B8BD56F-D6B6-4E47-8872-958781100D95}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1033,7 +1032,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8CB77162-68E2-4E3E-A1E2-D5A92D10E4AE}" type="CELLRANGE">
+                    <a:fld id="{51A53B35-23A0-4E87-8D71-C95D8C56484E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1067,7 +1066,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FB59897-748D-4437-A4E9-A6871B70A3DF}" type="CELLRANGE">
+                    <a:fld id="{01260916-6FB1-460E-86FA-C4E279361AE6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1101,7 +1100,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A513DD1C-BE6E-44D2-BD4D-0CCB01D34B6B}" type="CELLRANGE">
+                    <a:fld id="{40EFBEFF-CFD8-45D5-8524-961E34227D53}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1262,7 +1261,7 @@
                   <c:v>20440</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20557</c:v>
+                  <c:v>21370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1308,7 +1307,7 @@
                     <c:v>5.36%</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>5.36%</c:v>
+                    <c:v>5.33%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1837,7 +1836,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EC59E942-1512-46E5-B301-26CDCD03C741}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2176,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,32 +2589,32 @@
         <v>43739</v>
       </c>
       <c r="B13" s="1">
-        <v>117</v>
+        <v>930</v>
       </c>
       <c r="C13" s="6">
-        <v>3682</v>
+        <v>30315</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>2327</v>
+        <v>19239</v>
       </c>
       <c r="E13" s="3">
-        <v>2210</v>
+        <v>18309</v>
       </c>
       <c r="F13" s="3">
-        <v>6017</v>
+        <v>49582</v>
       </c>
       <c r="G13" s="3">
         <f>SUM(B$2:B13)</f>
-        <v>20557</v>
+        <v>21370</v>
       </c>
       <c r="H13" s="3">
         <f>SUM(D$2:D13)</f>
-        <v>383856</v>
+        <v>400768</v>
       </c>
       <c r="I13" s="5">
         <f>G13/H13</f>
-        <v>5.3553936893001544E-2</v>
+        <v>5.3322620568508464E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2710,15 +2709,15 @@
       </c>
       <c r="B30" s="3">
         <f>SUM(B2:B13)</f>
-        <v>20557</v>
+        <v>21370</v>
       </c>
       <c r="C30" s="3">
         <f>SUM(D2:D13)</f>
-        <v>383856</v>
+        <v>400768</v>
       </c>
       <c r="D30" s="3">
         <f>SUM(F2:F13)</f>
-        <v>1020352</v>
+        <v>1063917</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2727,11 +2726,11 @@
       </c>
       <c r="B31" s="5">
         <f>B30/C30</f>
-        <v>5.3553936893001544E-2</v>
+        <v>5.3322620568508464E-2</v>
       </c>
       <c r="C31" s="5">
         <f>100%-B31</f>
-        <v>0.94644606310699841</v>
+        <v>0.94667737943149155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit of Content/Home.htm,Content/Live use cases/Genes and health.htm,Content/Live use cases/NHS 111 Discovery frailty flagging.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png,Content/Use cases.htm
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7560DF5-B029-48FC-B8C7-04DDC627C333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ABA8A5-A9A1-4282-B436-10F4B8259037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B126A783-ABB5-4483-A304-7483DE945F42}" type="CELLRANGE">
+                    <a:fld id="{BB4C3FF8-90AB-4085-8E53-644FCA03356A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -760,7 +760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E14207AF-8DD4-4B73-A5B6-0B2A4B18414D}" type="CELLRANGE">
+                    <a:fld id="{E893BFD8-ECAE-4CA8-AC7A-45A3C47DBF63}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -794,7 +794,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5723B643-A9CC-478C-9EC0-DA2C1172391A}" type="CELLRANGE">
+                    <a:fld id="{6B71CC18-0D75-46E0-B3F1-59AA94D626BD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -828,7 +828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39E6D374-7606-4B4A-81EE-175B964CD421}" type="CELLRANGE">
+                    <a:fld id="{602CA9C5-110E-4806-9130-43737319E66B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -862,7 +862,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{731BE0BC-72D9-41B9-81EA-AD77CC6D4704}" type="CELLRANGE">
+                    <a:fld id="{E8E621C1-BCF1-449E-AB33-A12D8F121757}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -896,7 +896,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{761484A0-502E-4A79-ACE3-E320A5BE8006}" type="CELLRANGE">
+                    <a:fld id="{23CD0BAE-7B8C-40E2-BC66-F709C68E4C57}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -930,7 +930,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C78CF31-42FA-4658-A952-EE65697BFF53}" type="CELLRANGE">
+                    <a:fld id="{DF36D802-D903-4874-8673-9E20E2DFEB9E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -964,7 +964,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C34B9966-3200-42B6-8BA0-1F7483D2AF93}" type="CELLRANGE">
+                    <a:fld id="{95A4DCB6-3C27-48C4-B93B-584EA18C89EF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -998,7 +998,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B8BD56F-D6B6-4E47-8872-958781100D95}" type="CELLRANGE">
+                    <a:fld id="{4AED48F1-EFBA-48E1-AF64-F8B4E7739AA1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1032,7 +1032,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51A53B35-23A0-4E87-8D71-C95D8C56484E}" type="CELLRANGE">
+                    <a:fld id="{721730CE-DE25-41E6-ADE2-F3C4573F1018}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1066,7 +1066,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01260916-6FB1-460E-86FA-C4E279361AE6}" type="CELLRANGE">
+                    <a:fld id="{5E1219A0-59B2-4D48-BAE7-69AF82998824}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1100,7 +1100,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40EFBEFF-CFD8-45D5-8524-961E34227D53}" type="CELLRANGE">
+                    <a:fld id="{BCA2791B-822A-45BF-9951-308DB5E7A3DD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1261,7 +1261,7 @@
                   <c:v>20440</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21370</c:v>
+                  <c:v>22285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1307,7 +1307,7 @@
                     <c:v>5.36%</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>5.33%</c:v>
+                    <c:v>5.34%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2176,7 +2176,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,32 +2589,32 @@
         <v>43739</v>
       </c>
       <c r="B13" s="1">
-        <v>930</v>
+        <v>1845</v>
       </c>
       <c r="C13" s="6">
-        <v>30315</v>
+        <v>56912</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>19239</v>
+        <v>36143</v>
       </c>
       <c r="E13" s="3">
-        <v>18309</v>
+        <v>34298</v>
       </c>
       <c r="F13" s="3">
-        <v>49582</v>
+        <v>93074</v>
       </c>
       <c r="G13" s="3">
         <f>SUM(B$2:B13)</f>
-        <v>21370</v>
+        <v>22285</v>
       </c>
       <c r="H13" s="3">
         <f>SUM(D$2:D13)</f>
-        <v>400768</v>
+        <v>417672</v>
       </c>
       <c r="I13" s="5">
         <f>G13/H13</f>
-        <v>5.3322620568508464E-2</v>
+        <v>5.3355264418012222E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2709,15 +2709,15 @@
       </c>
       <c r="B30" s="3">
         <f>SUM(B2:B13)</f>
-        <v>21370</v>
+        <v>22285</v>
       </c>
       <c r="C30" s="3">
         <f>SUM(D2:D13)</f>
-        <v>400768</v>
+        <v>417672</v>
       </c>
       <c r="D30" s="3">
         <f>SUM(F2:F13)</f>
-        <v>1063917</v>
+        <v>1107409</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B31" s="5">
         <f>B30/C30</f>
-        <v>5.3322620568508464E-2</v>
+        <v>5.3355264418012222E-2</v>
       </c>
       <c r="C31" s="5">
         <f>100%-B31</f>
-        <v>0.94667737943149155</v>
+        <v>0.94664473558198781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit of Content/Live use cases/NHS 111 Discovery frailty flagging.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ABA8A5-A9A1-4282-B436-10F4B8259037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7E5BBF-6A71-46B0-BB13-2FBA888FA751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Matched and potentially not frail</t>
   </si>
@@ -64,6 +65,9 @@
   </si>
   <si>
     <t>Total API calls</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -726,8 +730,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB4C3FF8-90AB-4085-8E53-644FCA03356A}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{D0DDBAB5-BD64-4556-BCA7-70BC29301197}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -745,7 +749,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -760,8 +763,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E893BFD8-ECAE-4CA8-AC7A-45A3C47DBF63}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{2C549375-6EB9-4B5E-A01F-3238DA7F5C0C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -779,7 +782,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -794,8 +796,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B71CC18-0D75-46E0-B3F1-59AA94D626BD}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{1BB8252F-82D8-478C-93B0-D03BB9F956EF}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -813,7 +815,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -828,8 +829,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{602CA9C5-110E-4806-9130-43737319E66B}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{24669D75-6B8C-4D73-9C55-C274C4B1F39B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -847,7 +848,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -862,8 +862,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8E621C1-BCF1-449E-AB33-A12D8F121757}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{3170E351-7041-47BB-A6F9-FE1E97112FA1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -881,7 +881,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -896,8 +895,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23CD0BAE-7B8C-40E2-BC66-F709C68E4C57}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{E1727344-3A25-4B8D-BDC4-97EC6647F98C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -915,7 +914,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -930,8 +928,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF36D802-D903-4874-8673-9E20E2DFEB9E}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{569568CE-B40B-493A-B457-91B440262E61}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -949,7 +947,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -964,8 +961,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95A4DCB6-3C27-48C4-B93B-584EA18C89EF}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{C7BD5167-8E30-4144-B701-BCC1B2FB5139}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -983,7 +980,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -998,8 +994,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AED48F1-EFBA-48E1-AF64-F8B4E7739AA1}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{BD0BD001-3D7C-42F0-BFD2-726CA2BA66A1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1017,7 +1013,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1032,8 +1027,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{721730CE-DE25-41E6-ADE2-F3C4573F1018}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{14C23875-2368-483A-810A-0AE2BBD40486}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1051,7 +1046,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1066,8 +1060,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E1219A0-59B2-4D48-BAE7-69AF82998824}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{20F07168-2ADB-43B4-9133-0C3B36A5727D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1085,7 +1079,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1100,8 +1093,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCA2791B-822A-45BF-9951-308DB5E7A3DD}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{71FCF780-4936-4154-902D-46FD05FBB450}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1119,11 +1112,100 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-B051-4348-9DFB-0C03232B6B23}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1200" b="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{EF652235-93E2-4A0E-B0E3-5C194C6F6EA4}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr sz="1200" b="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="65000"/>
+                              <a:lumOff val="35000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                  <a:round/>
+                  <a:headEnd type="none" w="med" len="med"/>
+                  <a:tailEnd type="none" w="med" len="med"/>
+                  <a:extLst>
+                    <a:ext uri="{C807C97D-BFC1-408E-A445-0C87EB9F89A2}">
+                      <ask:lineSketchStyleProps xmlns:ask="http://schemas.microsoft.com/office/drawing/2018/sketchyshapes" sd="0">
+                        <a:custGeom>
+                          <a:avLst/>
+                          <a:gdLst/>
+                          <a:ahLst/>
+                          <a:cxnLst/>
+                          <a:rect l="0" t="0" r="0" b="0"/>
+                          <a:pathLst/>
+                        </a:custGeom>
+                        <ask:type/>
+                      </ask:lineSketchStyleProps>
+                    </a:ext>
+                  </a:extLst>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst>
+                        <a:gd name="adj1" fmla="val -2405"/>
+                        <a:gd name="adj2" fmla="val -34670"/>
+                      </a:avLst>
+                    </a:prstGeom>
+                  </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E0D1-4473-9599-EC4CF7B65D2F}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1144,8 +1226,8 @@
                   <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1178,10 +1260,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Totals!$A$2:$A$13</c:f>
+              <c:f>Totals!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43405</c:v>
                 </c:pt>
@@ -1218,15 +1300,18 @@
                 <c:pt idx="11">
                   <c:v>43739</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>43770</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Totals!$G$2:$G$13</c:f>
+              <c:f>Totals!$G$2:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>193</c:v>
                 </c:pt>
@@ -1261,7 +1346,10 @@
                   <c:v>20440</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22285</c:v>
+                  <c:v>22416</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,9 +1358,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Totals!$I$2:$I$13</c15:f>
+                <c15:f>Totals!$I$2:$I$14</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="12"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
                     <c:v>4.95%</c:v>
                   </c:pt>
@@ -1307,7 +1395,10 @@
                     <c:v>5.36%</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>5.34%</c:v>
+                    <c:v>5.33%</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5.41%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1429,13 +1520,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$13</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1471,6 +1562,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>43739</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>43770</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1599,13 +1693,13 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$13</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="13"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1641,6 +1735,9 @@
                       </c:pt>
                       <c:pt idx="11">
                         <c:v>43739</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>43770</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1836,7 +1933,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EC59E942-1512-46E5-B301-26CDCD03C741}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2173,10 +2270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2289,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2220,8 +2317,11 @@
       <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43405</v>
       </c>
@@ -2229,10 +2329,11 @@
         <v>193</v>
       </c>
       <c r="C2" s="3">
-        <v>5129</v>
+        <f>+D2</f>
+        <v>3899</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D13" si="0">E2+B2</f>
+        <f t="shared" ref="D2:D14" si="0">E2+B2</f>
         <v>3899</v>
       </c>
       <c r="E2" s="6">
@@ -2253,8 +2354,12 @@
         <f>G2/H2</f>
         <v>4.9499871761990256E-2</v>
       </c>
+      <c r="K2" s="3">
+        <f>C2+D2</f>
+        <v>7798</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43435</v>
       </c>
@@ -2286,8 +2391,12 @@
         <f t="shared" ref="I3:I12" si="1">G3/H3</f>
         <v>4.8837313499708768E-2</v>
       </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K14" si="2">C3+D3</f>
+        <v>95322</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43466</v>
       </c>
@@ -2319,8 +2428,12 @@
         <f t="shared" si="1"/>
         <v>4.7946185773579501E-2</v>
       </c>
+      <c r="K4" s="3">
+        <f t="shared" si="2"/>
+        <v>92279</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43497</v>
       </c>
@@ -2352,8 +2465,12 @@
         <f t="shared" si="1"/>
         <v>4.6351362544520831E-2</v>
       </c>
+      <c r="K5" s="3">
+        <f t="shared" si="2"/>
+        <v>88754</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43525</v>
       </c>
@@ -2385,8 +2502,12 @@
         <f t="shared" si="1"/>
         <v>4.7263071124283441E-2</v>
       </c>
+      <c r="K6" s="3">
+        <f t="shared" si="2"/>
+        <v>100655</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43556</v>
       </c>
@@ -2418,8 +2539,12 @@
         <f>G7/H7</f>
         <v>4.8763085202890723E-2</v>
       </c>
+      <c r="K7" s="3">
+        <f t="shared" si="2"/>
+        <v>103130</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43586</v>
       </c>
@@ -2451,8 +2576,12 @@
         <f t="shared" si="1"/>
         <v>5.0112686142763867E-2</v>
       </c>
+      <c r="K8" s="3">
+        <f t="shared" si="2"/>
+        <v>116882</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43617</v>
       </c>
@@ -2484,8 +2613,12 @@
         <f t="shared" si="1"/>
         <v>5.1706562366703054E-2</v>
       </c>
+      <c r="K9" s="3">
+        <f t="shared" si="2"/>
+        <v>110156</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43647</v>
       </c>
@@ -2517,8 +2650,12 @@
         <f>G10/H10</f>
         <v>5.2412399666067887E-2</v>
       </c>
+      <c r="K10" s="3">
+        <f t="shared" si="2"/>
+        <v>86332</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43678</v>
       </c>
@@ -2550,8 +2687,12 @@
         <f t="shared" si="1"/>
         <v>5.3842751362871304E-2</v>
       </c>
+      <c r="K11" s="3">
+        <f t="shared" si="2"/>
+        <v>110561</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43709</v>
       </c>
@@ -2583,52 +2724,92 @@
         <f t="shared" si="1"/>
         <v>5.3573909191699715E-2</v>
       </c>
+      <c r="K12" s="3">
+        <f t="shared" si="2"/>
+        <v>95900</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43739</v>
       </c>
       <c r="B13" s="1">
-        <v>1845</v>
+        <v>1976</v>
       </c>
       <c r="C13" s="6">
-        <v>56912</v>
+        <v>61290</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>36143</v>
+        <v>38770</v>
       </c>
       <c r="E13" s="3">
-        <v>34298</v>
+        <v>36794</v>
       </c>
       <c r="F13" s="3">
-        <v>93074</v>
+        <v>100088</v>
       </c>
       <c r="G13" s="3">
         <f>SUM(B$2:B13)</f>
-        <v>22285</v>
+        <v>22416</v>
       </c>
       <c r="H13" s="3">
         <f>SUM(D$2:D13)</f>
-        <v>417672</v>
+        <v>420299</v>
       </c>
       <c r="I13" s="5">
         <f>G13/H13</f>
-        <v>5.3355264418012222E-2</v>
+        <v>5.333346022712402E-2</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="2"/>
+        <v>100060</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43770</v>
       </c>
+      <c r="B14" s="1">
+        <v>2240</v>
+      </c>
+      <c r="C14" s="1">
+        <v>61279</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>35754</v>
+      </c>
+      <c r="E14" s="3">
+        <v>33514</v>
+      </c>
+      <c r="F14" s="3">
+        <v>97033</v>
+      </c>
+      <c r="G14" s="3">
+        <f>SUM(B$2:B14)</f>
+        <v>24656</v>
+      </c>
+      <c r="H14" s="3">
+        <f>SUM(D$2:D14)</f>
+        <v>456053</v>
+      </c>
+      <c r="I14" s="5">
+        <f>G14/H14</f>
+        <v>5.40638916967984E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="2"/>
+        <v>97033</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43800</v>
       </c>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43831</v>
       </c>
@@ -2708,16 +2889,16 @@
         <v>3</v>
       </c>
       <c r="B30" s="3">
-        <f>SUM(B2:B13)</f>
-        <v>22285</v>
+        <f>SUM(B2:B14)</f>
+        <v>24656</v>
       </c>
       <c r="C30" s="3">
-        <f>SUM(D2:D13)</f>
-        <v>417672</v>
+        <f>SUM(D2:D14)</f>
+        <v>456053</v>
       </c>
       <c r="D30" s="3">
-        <f>SUM(F2:F13)</f>
-        <v>1107409</v>
+        <f>SUM(F2:F14)</f>
+        <v>1211456</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,12 +2907,9 @@
       </c>
       <c r="B31" s="5">
         <f>B30/C30</f>
-        <v>5.3355264418012222E-2</v>
-      </c>
-      <c r="C31" s="5">
-        <f>100%-B31</f>
-        <v>0.94664473558198781</v>
-      </c>
+        <v>5.40638916967984E-2</v>
+      </c>
+      <c r="C31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit of Content/Live_use_cases/NHS_111_Discovery_frailty_flagging.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7E5BBF-6A71-46B0-BB13-2FBA888FA751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B67E31-B141-4DF3-B35F-3026931F7B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,22 +559,22 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -627,11 +627,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF79646"/>
       <color rgb="FF92D050"/>
       <color rgb="FF266196"/>
       <color rgb="FFFF6464"/>
       <color rgb="FF5B9BD5"/>
-      <color rgb="FFF79646"/>
       <color rgb="FF6600CC"/>
     </mruColors>
   </colors>
@@ -704,11 +704,11 @@
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="92D050"/>
+                <a:srgbClr val="F79646"/>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="92D050"/>
+                  <a:srgbClr val="F79646"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -730,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0DDBAB5-BD64-4556-BCA7-70BC29301197}" type="CELLRANGE">
+                    <a:fld id="{9E29F529-524E-4C64-B420-BC2FF95D1DEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -763,8 +763,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C549375-6EB9-4B5E-A01F-3238DA7F5C0C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{70DA2751-6A73-4F1E-9B83-7784E470B9FC}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -782,6 +782,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -796,8 +797,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BB8252F-82D8-478C-93B0-D03BB9F956EF}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D7571D40-D028-4B06-9BEB-7EBFB9824DF0}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -815,6 +816,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -829,8 +831,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24669D75-6B8C-4D73-9C55-C274C4B1F39B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{761EB423-02EC-4C92-9F98-B15E2E4455AB}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -848,6 +850,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -862,8 +865,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3170E351-7041-47BB-A6F9-FE1E97112FA1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4167B949-B176-4839-8D93-335829404251}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -881,6 +884,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -895,8 +899,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E1727344-3A25-4B8D-BDC4-97EC6647F98C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F962A1F1-DC30-4680-9645-B72A6DF3A9CA}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -914,6 +918,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -928,8 +933,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{569568CE-B40B-493A-B457-91B440262E61}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{A2B93200-6719-410A-ACD3-35230075668F}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -947,6 +952,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -961,8 +967,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7BD5167-8E30-4144-B701-BCC1B2FB5139}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{79D337D9-DED4-45A4-A1DB-61A6965FD83A}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -980,6 +986,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -994,8 +1001,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD0BD001-3D7C-42F0-BFD2-726CA2BA66A1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2915EB2F-FF5A-41B5-A355-02DB5D611202}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1013,6 +1020,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1027,8 +1035,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14C23875-2368-483A-810A-0AE2BBD40486}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7FE62F79-9C6A-4D1E-A578-FA2454E38389}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1046,6 +1054,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1060,8 +1069,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20F07168-2ADB-43B4-9133-0C3B36A5727D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7D8CFE64-F126-4F73-B81E-CF0B285A64DC}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1079,6 +1088,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1093,8 +1103,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71FCF780-4936-4154-902D-46FD05FBB450}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{EDA1F391-F54A-4423-B538-E2A31813D58E}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -1112,6 +1122,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1121,6 +1132,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.6092462597753681E-2"/>
+                  <c:y val="-3.220727503106003E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr rot="0" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050">
@@ -1138,7 +1155,7 @@
                         </a:solidFill>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{EF652235-93E2-4A0E-B0E3-5C194C6F6EA4}" type="CELLRANGE">
+                    <a:fld id="{E469E907-FFD1-4F05-8E1E-1AF3D0073877}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1200" b="1">
@@ -1157,9 +1174,7 @@
                 </c:rich>
               </c:tx>
               <c:spPr>
-                <a:solidFill>
-                  <a:sysClr val="window" lastClr="FFFFFF"/>
-                </a:solidFill>
+                <a:noFill/>
                 <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                   <a:noFill/>
                   <a:prstDash val="solid"/>
@@ -1184,7 +1199,7 @@
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1206,6 +1221,74 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-E0D1-4473-9599-EC4CF7B65D2F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{31B7C67C-88DC-434A-A4E1-2486967D1C79}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-DB16-4EB5-8A78-8A84DF169A60}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{207C6C9F-40E4-4FF7-8FD6-A133F3ED3116}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-DB16-4EB5-8A78-8A84DF169A60}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1260,10 +1343,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Totals!$A$2:$A$14</c:f>
+              <c:f>Totals!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43405</c:v>
                 </c:pt>
@@ -1303,15 +1386,21 @@
                 <c:pt idx="12">
                   <c:v>43770</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>43800</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43831</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Totals!$G$2:$G$14</c:f>
+              <c:f>Totals!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>193</c:v>
                 </c:pt>
@@ -1349,7 +1438,13 @@
                   <c:v>22416</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24656</c:v>
+                  <c:v>25213</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28638</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1358,9 +1453,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Totals!$I$2:$I$14</c15:f>
+                <c15:f>Totals!$I$2:$I$16</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="13"/>
+                  <c:ptCount val="15"/>
                   <c:pt idx="0">
                     <c:v>4.95%</c:v>
                   </c:pt>
@@ -1398,7 +1493,13 @@
                     <c:v>5.33%</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>5.41%</c:v>
+                    <c:v>5.43%</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>5.53%</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>5.56%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1520,13 +1621,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$14</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$16</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1565,6 +1666,12 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>43770</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>43800</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>43831</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1690,16 +1797,16 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$14</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$16</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1738,6 +1845,12 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>43770</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>43800</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>43831</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2273,19 +2386,19 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="34.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2302,10 +2415,10 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -2314,7 +2427,7 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -2322,565 +2435,624 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>43405</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>193</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>+D2</f>
         <v>3899</v>
       </c>
-      <c r="D2" s="3">
-        <f t="shared" ref="D2:D14" si="0">E2+B2</f>
+      <c r="D2" s="2">
+        <f t="shared" ref="D2:D16" si="0">E2+B2</f>
         <v>3899</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>3706</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>9028</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <f>SUM(B2:B$2)</f>
         <v>193</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <f>SUM(D2:D$2)</f>
         <v>3899</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <f>G2/H2</f>
         <v>4.9499871761990256E-2</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <f>C2+D2</f>
         <v>7798</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>43435</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1987</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>54583</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>40739</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>38752</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>95322</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f>SUM(B$2:B3)</f>
         <v>2180</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>SUM(D$2:D3)</f>
         <v>44638</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="6">
         <f t="shared" ref="I3:I12" si="1">G3/H3</f>
         <v>4.8837313499708768E-2</v>
       </c>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K14" si="2">C3+D3</f>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K16" si="2">C3+D3</f>
         <v>95322</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>43466</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1840</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>53073</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>39206</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>37366</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>92376</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>SUM(B$2:B4)</f>
         <v>4020</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f>SUM(D$2:D4)</f>
         <v>83844</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <f t="shared" si="1"/>
         <v>4.7946185773579501E-2</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <f t="shared" si="2"/>
         <v>92279</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>43497</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1576</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>51868</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>36886</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>35310</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>88754</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f>SUM(B$2:B5)</f>
         <v>5596</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f>SUM(D$2:D5)</f>
         <v>120730</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="6">
         <f t="shared" si="1"/>
         <v>4.6351362544520831E-2</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <f t="shared" si="2"/>
         <v>88754</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>43525</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1915</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>62466</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>38189</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>36274</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>100655</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f>SUM(B$2:B6)</f>
         <v>7511</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <f>SUM(D$2:D6)</f>
         <v>158919</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <f t="shared" si="1"/>
         <v>4.7263071124283441E-2</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <f t="shared" si="2"/>
         <v>100655</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>43556</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>2057</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>65835</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>37295</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>35238</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>103130</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f>SUM(B$2:B7)</f>
         <v>9568</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <f>SUM(D$2:D7)</f>
         <v>196214</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <f>G7/H7</f>
         <v>4.8763085202890723E-2</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
         <v>103130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>43586</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>2328</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>75711</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>41171</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>38843</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>116882</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f>SUM(B$2:B8)</f>
         <v>11896</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <f>SUM(D$2:D8)</f>
         <v>237385</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <f t="shared" si="1"/>
         <v>5.0112686142763867E-2</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
         <v>116882</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>43617</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>2408</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>70903</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>39253</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>36845</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>110156</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f>SUM(B$2:B9)</f>
         <v>14304</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <f>SUM(D$2:D9)</f>
         <v>276638</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
         <v>5.1706562366703054E-2</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
         <v>110156</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
         <v>43647</v>
       </c>
       <c r="B10" s="1">
         <v>1831</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>55123</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>31209</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>29378</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>86333</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f>SUM(B$2:B10)</f>
         <v>16135</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <f>SUM(D$2:D10)</f>
         <v>307847</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <f>G10/H10</f>
         <v>5.2412399666067887E-2</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
         <v>86332</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="4">
         <v>43678</v>
       </c>
       <c r="B11" s="1">
         <v>2611</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>70246</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>40315</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>37704</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>110572</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <f>SUM(B$2:B11)</f>
         <v>18746</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <f>SUM(D$2:D11)</f>
         <v>348162</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="6">
         <f t="shared" si="1"/>
         <v>5.3842751362871304E-2</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <f t="shared" si="2"/>
         <v>110561</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>43709</v>
       </c>
       <c r="B12" s="1">
         <v>1694</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>62533</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>33367</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>31673</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>101127</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <f>SUM(B$2:B12)</f>
         <v>20440</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <f>SUM(D$2:D12)</f>
         <v>381529</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="6">
         <f t="shared" si="1"/>
         <v>5.3573909191699715E-2</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <f t="shared" si="2"/>
         <v>95900</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="4">
         <v>43739</v>
       </c>
       <c r="B13" s="1">
         <v>1976</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>61290</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>38770</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>36794</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>100088</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f>SUM(B$2:B13)</f>
         <v>22416</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <f>SUM(D$2:D13)</f>
         <v>420299</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="6">
         <f>G13/H13</f>
         <v>5.333346022712402E-2</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="2">
         <f t="shared" si="2"/>
         <v>100060</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>43770</v>
       </c>
       <c r="B14" s="1">
-        <v>2240</v>
-      </c>
-      <c r="C14" s="1">
-        <v>61279</v>
-      </c>
-      <c r="D14" s="3">
+        <v>2797</v>
+      </c>
+      <c r="C14" s="5">
+        <v>75286</v>
+      </c>
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>35754</v>
-      </c>
-      <c r="E14" s="3">
-        <v>33514</v>
-      </c>
-      <c r="F14" s="3">
-        <v>97033</v>
-      </c>
-      <c r="G14" s="3">
+        <v>43999</v>
+      </c>
+      <c r="E14" s="2">
+        <v>41202</v>
+      </c>
+      <c r="F14" s="2">
+        <v>119285</v>
+      </c>
+      <c r="G14" s="2">
         <f>SUM(B$2:B14)</f>
-        <v>24656</v>
-      </c>
-      <c r="H14" s="3">
+        <v>25213</v>
+      </c>
+      <c r="H14" s="2">
         <f>SUM(D$2:D14)</f>
-        <v>456053</v>
-      </c>
-      <c r="I14" s="5">
+        <v>464298</v>
+      </c>
+      <c r="I14" s="6">
         <f>G14/H14</f>
-        <v>5.40638916967984E-2</v>
-      </c>
-      <c r="K14" s="3">
+        <v>5.4303486123136437E-2</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="2"/>
-        <v>97033</v>
+        <v>119285</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="4">
         <v>43800</v>
       </c>
-      <c r="B15"/>
+      <c r="B15" s="1">
+        <v>3425</v>
+      </c>
+      <c r="C15" s="5">
+        <v>87799</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>53459</v>
+      </c>
+      <c r="E15" s="2">
+        <v>50034</v>
+      </c>
+      <c r="F15" s="2">
+        <v>141258</v>
+      </c>
+      <c r="G15" s="2">
+        <f>SUM(B$2:B15)</f>
+        <v>28638</v>
+      </c>
+      <c r="H15" s="2">
+        <f>SUM(D$2:D15)</f>
+        <v>517757</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" ref="I15:I16" si="3">G15/H15</f>
+        <v>5.5311661648224937E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="2"/>
+        <v>141258</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="4">
         <v>43831</v>
       </c>
-      <c r="B16"/>
+      <c r="B16" s="1">
+        <v>675</v>
+      </c>
+      <c r="C16" s="5">
+        <v>16337</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>9847</v>
+      </c>
+      <c r="E16" s="2">
+        <v>9172</v>
+      </c>
+      <c r="F16" s="2">
+        <v>26184</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(B$2:B16)</f>
+        <v>29313</v>
+      </c>
+      <c r="H16" s="2">
+        <f>SUM(D$2:D16)</f>
+        <v>527604</v>
+      </c>
+      <c r="I16" s="6">
+        <f>G16/H16</f>
+        <v>5.5558714490413268E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="2"/>
+        <v>26184</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="4">
         <v>43862</v>
       </c>
-      <c r="B17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>43891</v>
       </c>
-      <c r="B18"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="4">
         <v>43922</v>
       </c>
-      <c r="B19"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="4">
         <v>43952</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="4">
         <v>43983</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="4">
         <v>44013</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="4">
         <v>44044</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="4">
         <v>44075</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="4">
         <v>44105</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="4">
         <v>44136</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="4">
         <v>44166</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2888,28 +3060,28 @@
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="3">
-        <f>SUM(B2:B14)</f>
-        <v>24656</v>
-      </c>
-      <c r="C30" s="3">
-        <f>SUM(D2:D14)</f>
-        <v>456053</v>
-      </c>
-      <c r="D30" s="3">
-        <f>SUM(F2:F14)</f>
-        <v>1211456</v>
+      <c r="B30" s="2">
+        <f>SUM(B2:B27)</f>
+        <v>29313</v>
+      </c>
+      <c r="C30" s="2">
+        <f>SUM(D2:D27)</f>
+        <v>527604</v>
+      </c>
+      <c r="D30" s="2">
+        <f>SUM(F2:F27)</f>
+        <v>1401150</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <f>B30/C30</f>
-        <v>5.40638916967984E-2</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>5.5558714490413268E-2</v>
+      </c>
+      <c r="C31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit of Content/Documentation.htm,Content/Live_use_cases/Genes_and_health.htm,Content/Live_use_cases/NHS_111_Discovery_frailty_flagging.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/DDS publishers.png,Content/Resources/Images/Frailty graph.png,Content/Resources/Images/Logos/East London genes and health.jpg,Content/Specs/Discovery_Data_Model.htm,Content/Specs/Language and structural specification.htm,Content/Technical.htm
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B67E31-B141-4DF3-B35F-3026931F7B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5353F7C3-03E8-45BB-B80E-5BDD882A9FC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
@@ -730,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E29F529-524E-4C64-B420-BC2FF95D1DEC}" type="CELLRANGE">
+                    <a:fld id="{39ABAEE6-E0D4-425B-9E93-02543DD0DDEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -763,7 +763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70DA2751-6A73-4F1E-9B83-7784E470B9FC}" type="CELLRANGE">
+                    <a:fld id="{6884D5A9-1618-4135-9B65-197E7928A04C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -797,7 +797,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7571D40-D028-4B06-9BEB-7EBFB9824DF0}" type="CELLRANGE">
+                    <a:fld id="{8BDD950A-9BEC-4C30-9B8C-26C6FBC711A2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -831,7 +831,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{761EB423-02EC-4C92-9F98-B15E2E4455AB}" type="CELLRANGE">
+                    <a:fld id="{54C0CCAB-E3F7-4C85-8600-852691577102}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -865,7 +865,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4167B949-B176-4839-8D93-335829404251}" type="CELLRANGE">
+                    <a:fld id="{8179B9D9-4AB3-455B-9251-0FC4ED569ABE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -899,7 +899,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F962A1F1-DC30-4680-9645-B72A6DF3A9CA}" type="CELLRANGE">
+                    <a:fld id="{EF64DD6A-1427-4CEB-9306-6E7DC80FA351}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -933,7 +933,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2B93200-6719-410A-ACD3-35230075668F}" type="CELLRANGE">
+                    <a:fld id="{572C8249-C9EC-4560-820E-7DB2B15634EC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -967,7 +967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79D337D9-DED4-45A4-A1DB-61A6965FD83A}" type="CELLRANGE">
+                    <a:fld id="{5D3511FB-A960-40B1-B6C4-FE93E1F50278}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1001,7 +1001,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2915EB2F-FF5A-41B5-A355-02DB5D611202}" type="CELLRANGE">
+                    <a:fld id="{F998F42C-6B20-4D45-B2FD-3A5ED6BAFF2D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1035,7 +1035,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FE62F79-9C6A-4D1E-A578-FA2454E38389}" type="CELLRANGE">
+                    <a:fld id="{F1BC2E7E-D4F4-4FD5-90AE-40CCCA87FE1B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1069,7 +1069,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D8CFE64-F126-4F73-B81E-CF0B285A64DC}" type="CELLRANGE">
+                    <a:fld id="{D15D4AB2-5C03-4174-83AA-F338D5BC233C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1103,7 +1103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDA1F391-F54A-4423-B538-E2A31813D58E}" type="CELLRANGE">
+                    <a:fld id="{C7F25633-EC8A-4252-AD7E-720A6BE88E59}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1155,7 +1155,7 @@
                         </a:solidFill>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{E469E907-FFD1-4F05-8E1E-1AF3D0073877}" type="CELLRANGE">
+                    <a:fld id="{364B9302-2FD0-4ED3-81BF-EC86B93B12B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1200" b="1">
@@ -1231,7 +1231,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31B7C67C-88DC-434A-A4E1-2486967D1C79}" type="CELLRANGE">
+                    <a:fld id="{73F1C2EC-B3A5-451A-AC11-B41584CEC537}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1265,7 +1265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{207C6C9F-40E4-4FF7-8FD6-A133F3ED3116}" type="CELLRANGE">
+                    <a:fld id="{032F54BB-3523-4952-9D33-D63652D1C85F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1444,7 +1444,7 @@
                   <c:v>28638</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29313</c:v>
+                  <c:v>31972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1499,7 +1499,7 @@
                     <c:v>5.53%</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>5.56%</c:v>
+                    <c:v>5.65%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1797,7 +1797,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Totals!$A$2:$A$16</c15:sqref>
@@ -2046,7 +2046,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EC59E942-1512-46E5-B301-26CDCD03C741}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2385,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,7 +2446,7 @@
         <v>3899</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D16" si="0">E2+B2</f>
+        <f t="shared" ref="D2:D17" si="0">E2+B2</f>
         <v>3899</v>
       </c>
       <c r="E2" s="5">
@@ -2945,7 +2945,7 @@
         <v>517757</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" ref="I15:I16" si="3">G15/H15</f>
+        <f t="shared" ref="I15" si="3">G15/H15</f>
         <v>5.5311661648224937E-2</v>
       </c>
       <c r="K15" s="2">
@@ -2958,94 +2958,126 @@
         <v>43831</v>
       </c>
       <c r="B16" s="1">
-        <v>675</v>
+        <v>3334</v>
       </c>
       <c r="C16" s="5">
-        <v>16337</v>
+        <v>81573</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>9847</v>
+        <v>47843</v>
       </c>
       <c r="E16" s="2">
-        <v>9172</v>
+        <v>44509</v>
       </c>
       <c r="F16" s="2">
-        <v>26184</v>
+        <v>129416</v>
       </c>
       <c r="G16" s="2">
         <f>SUM(B$2:B16)</f>
-        <v>29313</v>
+        <v>31972</v>
       </c>
       <c r="H16" s="2">
         <f>SUM(D$2:D16)</f>
-        <v>527604</v>
+        <v>565600</v>
       </c>
       <c r="I16" s="6">
         <f>G16/H16</f>
-        <v>5.5558714490413268E-2</v>
+        <v>5.6527581329561524E-2</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="2"/>
-        <v>26184</v>
+        <v>129416</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43862</v>
       </c>
+      <c r="B17" s="1">
+        <v>352</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10497</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>6201</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5849</v>
+      </c>
+      <c r="F17" s="2">
+        <v>16698</v>
+      </c>
+      <c r="G17" s="2">
+        <f>SUM(B$2:B17)</f>
+        <v>32324</v>
+      </c>
+      <c r="H17" s="2">
+        <f>SUM(D$2:D17)</f>
+        <v>571801</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" ref="I17" si="4">G17/H17</f>
+        <v>5.6530156470520336E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" ref="K17" si="5">C17+D17</f>
+        <v>16698</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43891</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43922</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43952</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43983</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>44013</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>44044</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>44075</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>44105</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>44136</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>44166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
@@ -3056,30 +3088,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="2">
         <f>SUM(B2:B27)</f>
-        <v>29313</v>
+        <v>32324</v>
       </c>
       <c r="C30" s="2">
         <f>SUM(D2:D27)</f>
-        <v>527604</v>
+        <v>571801</v>
       </c>
       <c r="D30" s="2">
         <f>SUM(F2:F27)</f>
-        <v>1401150</v>
+        <v>1521080</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="6">
         <f>B30/C30</f>
-        <v>5.5558714490413268E-2</v>
+        <v>5.6530156470520336E-2</v>
       </c>
       <c r="C31" s="6"/>
     </row>

</xml_diff>

<commit_message>
Commit of Content/Live_use_cases/NHS_111_Discovery_frailty_flagging.htm,Content/Popups/Frailty_graph.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png,Project/Targets/HTML5 - Top Navigation.fltar
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5353F7C3-03E8-45BB-B80E-5BDD882A9FC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB9D6A-F3B8-4266-94EB-60090A585B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12696" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
@@ -627,8 +627,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF92D050"/>
       <color rgb="FFF79646"/>
-      <color rgb="FF92D050"/>
       <color rgb="FF266196"/>
       <color rgb="FFFF6464"/>
       <color rgb="FF5B9BD5"/>
@@ -704,11 +704,11 @@
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="F79646"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="F79646"/>
+                  <a:srgbClr val="92D050"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -730,8 +730,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39ABAEE6-E0D4-425B-9E93-02543DD0DDEA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{AC839B0C-44CE-478C-9EEA-EEBC7C8FE1B4}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -739,7 +739,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -749,6 +749,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -763,7 +764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6884D5A9-1618-4135-9B65-197E7928A04C}" type="CELLRANGE">
+                    <a:fld id="{BDA10782-0415-42D3-A0CF-9B4334416AAB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -772,7 +773,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -797,7 +798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BDD950A-9BEC-4C30-9B8C-26C6FBC711A2}" type="CELLRANGE">
+                    <a:fld id="{A3424F91-0DF5-4F0E-AE6B-38CF5A90B3E3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -806,7 +807,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -831,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54C0CCAB-E3F7-4C85-8600-852691577102}" type="CELLRANGE">
+                    <a:fld id="{7EB9ED79-4AC3-409A-88F9-8E4AFFBDB0BA}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -840,7 +841,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -865,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8179B9D9-4AB3-455B-9251-0FC4ED569ABE}" type="CELLRANGE">
+                    <a:fld id="{BE56140D-182E-4647-9C30-298E99E352AF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -874,7 +875,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -899,7 +900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF64DD6A-1427-4CEB-9306-6E7DC80FA351}" type="CELLRANGE">
+                    <a:fld id="{E7A11D15-0C9F-4A08-9C0F-A6A564811572}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -908,7 +909,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -933,7 +934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{572C8249-C9EC-4560-820E-7DB2B15634EC}" type="CELLRANGE">
+                    <a:fld id="{1BF3D349-0E28-4152-B0AB-B30E1982B088}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -942,7 +943,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -967,7 +968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D3511FB-A960-40B1-B6C4-FE93E1F50278}" type="CELLRANGE">
+                    <a:fld id="{D7963302-E2C6-479C-B0E2-B138AB65D383}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -976,7 +977,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1001,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F998F42C-6B20-4D45-B2FD-3A5ED6BAFF2D}" type="CELLRANGE">
+                    <a:fld id="{342730BB-F683-4470-A85B-01F1C6B91106}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1010,7 +1011,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1035,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1BC2E7E-D4F4-4FD5-90AE-40CCCA87FE1B}" type="CELLRANGE">
+                    <a:fld id="{7AF1505C-68EE-40D4-8F5D-6C6C6FBFCB01}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1044,7 +1045,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1069,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D15D4AB2-5C03-4174-83AA-F338D5BC233C}" type="CELLRANGE">
+                    <a:fld id="{C32CFC8F-A19D-4BAA-897C-B142C79EFAB2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1078,7 +1079,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1103,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7F25633-EC8A-4252-AD7E-720A6BE88E59}" type="CELLRANGE">
+                    <a:fld id="{8B6847B7-C021-4601-90CF-71370028FC7A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1112,7 +1113,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1132,15 +1133,9 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.6092462597753681E-2"/>
-                  <c:y val="-3.220727503106003E-2"/>
-                </c:manualLayout>
-              </c:layout>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+                  <a:bodyPr rot="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="108000" tIns="144000" rIns="144000" bIns="0" anchor="b" anchorCtr="1">
                     <a:spAutoFit/>
                   </a:bodyPr>
                   <a:lstStyle/>
@@ -1155,8 +1150,8 @@
                         </a:solidFill>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{364B9302-2FD0-4ED3-81BF-EC86B93B12B3}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{59F52B16-1F86-4A19-8339-7E3286DDAE1A}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="1200" b="1">
                           <a:solidFill>
@@ -1217,6 +1212,7 @@
                     </a:prstGeom>
                   </c15:spPr>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1231,7 +1227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73F1C2EC-B3A5-451A-AC11-B41584CEC537}" type="CELLRANGE">
+                    <a:fld id="{340682AA-F753-4DC8-B996-77F407D4C50C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1240,7 +1236,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1265,7 +1261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{032F54BB-3523-4952-9D33-D63652D1C85F}" type="CELLRANGE">
+                    <a:fld id="{B90C538A-AA4B-467A-88B9-48C3F6ECCA08}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1274,7 +1270,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="t"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1292,6 +1288,40 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FC244336-865A-4DD3-8908-47452ADE5494}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-FD32-4578-AB05-9920D1D5FFBC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1300,7 +1330,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="0" rIns="252000" bIns="0" anchor="t" anchorCtr="0">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="108000" tIns="144000" rIns="144000" bIns="0" anchor="b" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1321,7 +1351,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1343,10 +1373,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Totals!$A$2:$A$16</c:f>
+              <c:f>Totals!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>43405</c:v>
                 </c:pt>
@@ -1391,16 +1421,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>43831</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Totals!$G$2:$G$16</c:f>
+              <c:f>Totals!$G$2:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>193</c:v>
                 </c:pt>
@@ -1445,6 +1478,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>31972</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,9 +1489,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Totals!$I$2:$I$16</c15:f>
+                <c15:f>Totals!$I$2:$I$17</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="15"/>
+                  <c:ptCount val="16"/>
                   <c:pt idx="0">
                     <c:v>4.95%</c:v>
                   </c:pt>
@@ -1499,6 +1535,9 @@
                     <c:v>5.53%</c:v>
                   </c:pt>
                   <c:pt idx="14">
+                    <c:v>5.65%</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>5.65%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -1621,13 +1660,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$16</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="16"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1672,6 +1711,9 @@
                       </c:pt>
                       <c:pt idx="14">
                         <c:v>43831</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>43862</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1797,16 +1839,16 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$16</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="16"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1851,6 +1893,9 @@
                       </c:pt>
                       <c:pt idx="14">
                         <c:v>43831</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>43862</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1935,7 +1980,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="679110136"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
@@ -2046,7 +2091,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EC59E942-1512-46E5-B301-26CDCD03C741}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2057,7 +2102,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305925" cy="6076950"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2081,7 +2126,7 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0" fPrintsWithSheet="0"/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
@@ -2385,24 +2430,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.41796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2434,7 +2479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>43405</v>
       </c>
@@ -2472,7 +2517,7 @@
         <v>7798</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4">
         <v>43435</v>
       </c>
@@ -2509,7 +2554,7 @@
         <v>95322</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>43466</v>
       </c>
@@ -2546,7 +2591,7 @@
         <v>92279</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4">
         <v>43497</v>
       </c>
@@ -2583,7 +2628,7 @@
         <v>88754</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>43525</v>
       </c>
@@ -2620,7 +2665,7 @@
         <v>100655</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>43556</v>
       </c>
@@ -2657,7 +2702,7 @@
         <v>103130</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>43586</v>
       </c>
@@ -2694,7 +2739,7 @@
         <v>116882</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4">
         <v>43617</v>
       </c>
@@ -2731,11 +2776,11 @@
         <v>110156</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
         <v>43647</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>1831</v>
       </c>
       <c r="C10" s="5">
@@ -2768,11 +2813,11 @@
         <v>86332</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4">
         <v>43678</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>2611</v>
       </c>
       <c r="C11" s="5">
@@ -2805,11 +2850,11 @@
         <v>110561</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4">
         <v>43709</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>1694</v>
       </c>
       <c r="C12" s="5">
@@ -2842,11 +2887,11 @@
         <v>95900</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4">
         <v>43739</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>1976</v>
       </c>
       <c r="C13" s="5">
@@ -2879,11 +2924,11 @@
         <v>100060</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4">
         <v>43770</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>2797</v>
       </c>
       <c r="C14" s="5">
@@ -2916,11 +2961,11 @@
         <v>119285</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4">
         <v>43800</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>3425</v>
       </c>
       <c r="C15" s="5">
@@ -2953,11 +2998,11 @@
         <v>141258</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4">
         <v>43831</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>3334</v>
       </c>
       <c r="C16" s="5">
@@ -2990,94 +3035,94 @@
         <v>129416</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4">
         <v>43862</v>
       </c>
-      <c r="B17" s="1">
-        <v>352</v>
-      </c>
-      <c r="C17" s="1">
-        <v>10497</v>
+      <c r="B17" s="2">
+        <v>2749</v>
+      </c>
+      <c r="C17" s="5">
+        <v>83167</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>6201</v>
+        <v>48622</v>
       </c>
       <c r="E17" s="2">
-        <v>5849</v>
+        <v>45873</v>
       </c>
       <c r="F17" s="2">
-        <v>16698</v>
+        <v>131789</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(B$2:B17)</f>
-        <v>32324</v>
+        <v>34721</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(D$2:D17)</f>
-        <v>571801</v>
+        <v>614222</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" ref="I17" si="4">G17/H17</f>
-        <v>5.6530156470520336E-2</v>
+        <v>5.6528421319978768E-2</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" ref="K17" si="5">C17+D17</f>
-        <v>16698</v>
+        <v>131789</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>43891</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4">
         <v>43922</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>43952</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4">
         <v>43983</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>44013</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4">
         <v>44044</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
         <v>44075</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4">
         <v>44105</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4">
         <v>44136</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4">
         <v>44166</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
@@ -3088,30 +3133,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="2">
         <f>SUM(B2:B27)</f>
-        <v>32324</v>
+        <v>34721</v>
       </c>
       <c r="C30" s="2">
         <f>SUM(D2:D27)</f>
-        <v>571801</v>
+        <v>614222</v>
       </c>
       <c r="D30" s="2">
         <f>SUM(F2:F27)</f>
-        <v>1521080</v>
+        <v>1636171</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="6">
         <f>B30/C30</f>
-        <v>5.6530156470520336E-2</v>
+        <v>5.6528421319978768E-2</v>
       </c>
       <c r="C31" s="6"/>
     </row>

</xml_diff>

<commit_message>
Commit of Content/Live_use_cases/NHS_111_Discovery_frailty_flagging.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png,Content/Technical.htm
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB9D6A-F3B8-4266-94EB-60090A585B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067B2673-3525-4440-9CE2-8E365995AEF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12696" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
@@ -627,10 +627,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF79646"/>
+      <color rgb="FFFF6464"/>
       <color rgb="FF92D050"/>
-      <color rgb="FFF79646"/>
       <color rgb="FF266196"/>
-      <color rgb="FFFF6464"/>
       <color rgb="FF5B9BD5"/>
       <color rgb="FF6600CC"/>
     </mruColors>
@@ -704,11 +704,11 @@
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="92D050"/>
+                <a:srgbClr val="F79646"/>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="92D050"/>
+                  <a:srgbClr val="F79646"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -730,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC839B0C-44CE-478C-9EEA-EEBC7C8FE1B4}" type="CELLRANGE">
+                    <a:fld id="{2CB59BC9-BBEC-4912-BBCB-DB698D4D8AAC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -764,7 +764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BDA10782-0415-42D3-A0CF-9B4334416AAB}" type="CELLRANGE">
+                    <a:fld id="{258194BB-E528-4357-B1CF-40F4C9E5D571}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -798,7 +798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3424F91-0DF5-4F0E-AE6B-38CF5A90B3E3}" type="CELLRANGE">
+                    <a:fld id="{18196A0F-6108-4790-9E04-B4CD1CF57DCE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -832,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EB9ED79-4AC3-409A-88F9-8E4AFFBDB0BA}" type="CELLRANGE">
+                    <a:fld id="{5C6D89DC-D283-499F-B354-C189A7D134C2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -866,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE56140D-182E-4647-9C30-298E99E352AF}" type="CELLRANGE">
+                    <a:fld id="{34912168-6470-4798-AEB5-EB92B69C56C2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -900,7 +900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7A11D15-0C9F-4A08-9C0F-A6A564811572}" type="CELLRANGE">
+                    <a:fld id="{58A710C2-762E-4506-A038-27DCEDD51C21}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -934,7 +934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BF3D349-0E28-4152-B0AB-B30E1982B088}" type="CELLRANGE">
+                    <a:fld id="{42E1424B-6857-4864-9BAD-2A63EFDF2D08}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -968,7 +968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7963302-E2C6-479C-B0E2-B138AB65D383}" type="CELLRANGE">
+                    <a:fld id="{74B40448-F417-44FF-BB4D-40D2E0A2BB30}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1002,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{342730BB-F683-4470-A85B-01F1C6B91106}" type="CELLRANGE">
+                    <a:fld id="{E15671B7-31E1-4655-996F-F683BFFCD1E4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1036,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AF1505C-68EE-40D4-8F5D-6C6C6FBFCB01}" type="CELLRANGE">
+                    <a:fld id="{3308D2F2-B1C1-43ED-AD14-F11E7EFE1C65}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1070,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C32CFC8F-A19D-4BAA-897C-B142C79EFAB2}" type="CELLRANGE">
+                    <a:fld id="{4D4D5089-6E91-49C9-8EE5-EF9FA428E866}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1104,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B6847B7-C021-4601-90CF-71370028FC7A}" type="CELLRANGE">
+                    <a:fld id="{CC4DFB51-7087-408E-BE7B-5C26F3D7EB7B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1150,7 +1150,7 @@
                         </a:solidFill>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{59F52B16-1F86-4A19-8339-7E3286DDAE1A}" type="CELLRANGE">
+                    <a:fld id="{A5297C10-5AE7-41B9-A9C2-510BE8700350}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="1200" b="1">
@@ -1227,7 +1227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{340682AA-F753-4DC8-B996-77F407D4C50C}" type="CELLRANGE">
+                    <a:fld id="{F898D18F-5A5F-4E8D-A863-0FC23AACA96E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1261,7 +1261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B90C538A-AA4B-467A-88B9-48C3F6ECCA08}" type="CELLRANGE">
+                    <a:fld id="{6D30A8F4-9C8A-4AB8-BA48-31243B010726}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1295,7 +1295,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC244336-865A-4DD3-8908-47452ADE5494}" type="CELLRANGE">
+                    <a:fld id="{F015EE22-4E4A-4448-8F13-7FA051F5F19F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1319,6 +1319,74 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-FD32-4578-AB05-9920D1D5FFBC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2637F486-3A3B-4849-BCA3-0B150EECB720}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1708-46C1-B690-ADE91B0FA46B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AF9B3F25-8B00-46F2-956E-E47B80F867C2}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-1708-46C1-B690-ADE91B0FA46B}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1373,10 +1441,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Totals!$A$2:$A$17</c:f>
+              <c:f>Totals!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>43405</c:v>
                 </c:pt>
@@ -1424,16 +1492,22 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Totals!$G$2:$G$17</c:f>
+              <c:f>Totals!$G$2:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>193</c:v>
                 </c:pt>
@@ -1481,6 +1555,12 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>34721</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37378</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39091</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1489,9 +1569,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Totals!$I$2:$I$17</c15:f>
+                <c15:f>Totals!$I$2:$I$19</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="16"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>4.95%</c:v>
                   </c:pt>
@@ -1539,6 +1619,12 @@
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>5.65%</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>5.58%</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>5.62%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1660,13 +1746,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$17</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$19</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="16"/>
+                      <c:ptCount val="18"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1714,6 +1800,12 @@
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>43862</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>43891</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>43922</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1842,13 +1934,13 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Totals!$A$2:$A$17</c15:sqref>
+                          <c15:sqref>Totals!$A$2:$A$19</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="16"/>
+                      <c:ptCount val="18"/>
                       <c:pt idx="0">
                         <c:v>43405</c:v>
                       </c:pt>
@@ -1896,6 +1988,12 @@
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>43862</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>43891</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>43922</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2102,7 +2200,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9296400" cy="6070600"/>
+    <xdr:ext cx="9305925" cy="6076950"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2430,24 +2528,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="34.41796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.68359375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2479,7 +2577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43405</v>
       </c>
@@ -2491,7 +2589,7 @@
         <v>3899</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D17" si="0">E2+B2</f>
+        <f t="shared" ref="D2:D19" si="0">E2+B2</f>
         <v>3899</v>
       </c>
       <c r="E2" s="5">
@@ -2517,7 +2615,7 @@
         <v>7798</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43435</v>
       </c>
@@ -2554,7 +2652,7 @@
         <v>95322</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43466</v>
       </c>
@@ -2591,7 +2689,7 @@
         <v>92279</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43497</v>
       </c>
@@ -2628,7 +2726,7 @@
         <v>88754</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43525</v>
       </c>
@@ -2665,7 +2763,7 @@
         <v>100655</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43556</v>
       </c>
@@ -2702,7 +2800,7 @@
         <v>103130</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43586</v>
       </c>
@@ -2739,7 +2837,7 @@
         <v>116882</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43617</v>
       </c>
@@ -2776,7 +2874,7 @@
         <v>110156</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43647</v>
       </c>
@@ -2813,7 +2911,7 @@
         <v>86332</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43678</v>
       </c>
@@ -2850,7 +2948,7 @@
         <v>110561</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43709</v>
       </c>
@@ -2887,7 +2985,7 @@
         <v>95900</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43739</v>
       </c>
@@ -2924,7 +3022,7 @@
         <v>100060</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43770</v>
       </c>
@@ -2961,7 +3059,7 @@
         <v>119285</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43800</v>
       </c>
@@ -2998,7 +3096,7 @@
         <v>141258</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43831</v>
       </c>
@@ -3035,7 +3133,7 @@
         <v>129416</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43862</v>
       </c>
@@ -3064,65 +3162,129 @@
         <v>614222</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" ref="I17" si="4">G17/H17</f>
+        <f t="shared" ref="I17:I18" si="4">G17/H17</f>
         <v>5.6528421319978768E-2</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17" si="5">C17+D17</f>
+        <f t="shared" ref="K17:K19" si="5">C17+D17</f>
         <v>131789</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43891</v>
       </c>
+      <c r="B18" s="2">
+        <v>2657</v>
+      </c>
+      <c r="C18" s="5">
+        <v>95521</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>56120</v>
+      </c>
+      <c r="E18" s="2">
+        <v>53463</v>
+      </c>
+      <c r="F18" s="2">
+        <v>151642</v>
+      </c>
+      <c r="G18" s="2">
+        <f>SUM(B$2:B18)</f>
+        <v>37378</v>
+      </c>
+      <c r="H18" s="2">
+        <f>SUM(D$2:D18)</f>
+        <v>670342</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="4"/>
+        <v>5.5759597339865324E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="5"/>
+        <v>151641</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43922</v>
       </c>
+      <c r="B19" s="2">
+        <v>1713</v>
+      </c>
+      <c r="C19" s="5">
+        <v>38371</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>24762</v>
+      </c>
+      <c r="E19" s="2">
+        <v>23049</v>
+      </c>
+      <c r="F19" s="2">
+        <v>63133</v>
+      </c>
+      <c r="G19" s="2">
+        <f>SUM(B$2:B19)</f>
+        <v>39091</v>
+      </c>
+      <c r="H19" s="2">
+        <f>SUM(D$2:D19)</f>
+        <v>695104</v>
+      </c>
+      <c r="I19" s="6">
+        <f>G19/H19</f>
+        <v>5.6237627750667527E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="5"/>
+        <v>63133</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43952</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43983</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>44013</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>44044</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>44075</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>44105</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>44136</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>44166</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
@@ -3133,30 +3295,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="2">
         <f>SUM(B2:B27)</f>
-        <v>34721</v>
+        <v>39091</v>
       </c>
       <c r="C30" s="2">
         <f>SUM(D2:D27)</f>
-        <v>614222</v>
+        <v>695104</v>
       </c>
       <c r="D30" s="2">
         <f>SUM(F2:F27)</f>
-        <v>1636171</v>
+        <v>1850946</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="6">
         <f>B30/C30</f>
-        <v>5.6528421319978768E-2</v>
+        <v>5.6237627750667527E-2</v>
       </c>
       <c r="C31" s="6"/>
     </row>

</xml_diff>

<commit_message>
Commit of Content/Live_use_cases/NHS_111_Discovery_frailty_flagging.htm,Content/Resources/frailty codes.xlsx,Content/Resources/Images/Frailty graph.png,Content/Technical.htm,Project/Targets/HTML5 - Top Navigation.fltar
</commit_message>
<xml_diff>
--- a/Content/Resources/frailty codes.xlsx
+++ b/Content/Resources/frailty codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\Documents\My Projects\Discovery Data Service\Content\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067B2673-3525-4440-9CE2-8E365995AEF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192D6ABE-975E-44F2-8F3F-AEBE9EAB8B84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15990" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" tabRatio="212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frailty graph" sheetId="9" r:id="rId1"/>
@@ -730,7 +730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CB59BC9-BBEC-4912-BBCB-DB698D4D8AAC}" type="CELLRANGE">
+                    <a:fld id="{41DCA143-B8F7-40B9-99D5-F44B09F506E0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -764,7 +764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{258194BB-E528-4357-B1CF-40F4C9E5D571}" type="CELLRANGE">
+                    <a:fld id="{C5A6F405-E999-4CCC-ADFA-B4A6C9702CBB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -798,7 +798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18196A0F-6108-4790-9E04-B4CD1CF57DCE}" type="CELLRANGE">
+                    <a:fld id="{F6EAC10A-0A6A-4D60-9710-913C85B4F3E2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -832,7 +832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C6D89DC-D283-499F-B354-C189A7D134C2}" type="CELLRANGE">
+                    <a:fld id="{E3E55BD9-5BFC-41D5-8530-C4B08AE062EC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -866,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34912168-6470-4798-AEB5-EB92B69C56C2}" type="CELLRANGE">
+                    <a:fld id="{456D1F04-AE3A-4F8C-88DB-7F17AE53D9AC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -900,7 +900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58A710C2-762E-4506-A038-27DCEDD51C21}" type="CELLRANGE">
+                    <a:fld id="{8CB67280-8607-4832-8569-FC17D6A3ED39}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -934,7 +934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42E1424B-6857-4864-9BAD-2A63EFDF2D08}" type="CELLRANGE">
+                    <a:fld id="{26D841A4-0374-419C-B7F6-98CABAA3B9CB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -968,7 +968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74B40448-F417-44FF-BB4D-40D2E0A2BB30}" type="CELLRANGE">
+                    <a:fld id="{BCB9808B-37FE-496D-A4DC-A979B3ACE8F1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1002,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E15671B7-31E1-4655-996F-F683BFFCD1E4}" type="CELLRANGE">
+                    <a:fld id="{83FC007B-D7A4-4C7A-B8FD-C55688352060}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1036,7 +1036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3308D2F2-B1C1-43ED-AD14-F11E7EFE1C65}" type="CELLRANGE">
+                    <a:fld id="{3156705A-0570-47C7-849E-A95C4951873D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1070,7 +1070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D4D5089-6E91-49C9-8EE5-EF9FA428E866}" type="CELLRANGE">
+                    <a:fld id="{42F3D799-0189-4FE1-AD24-0E17BF3EA53A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1104,7 +1104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC4DFB51-7087-408E-BE7B-5C26F3D7EB7B}" type="CELLRANGE">
+                    <a:fld id="{6CBC9A0A-5380-476C-BB1F-A9FD78E4C4F9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1150,7 +1150,7 @@
                         </a:solidFill>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{A5297C10-5AE7-41B9-A9C2-510BE8700350}" type="CELLRANGE">
+                    <a:fld id="{2864FE3B-1894-4977-8D9C-9D03F5C5A26B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="1200" b="1">
@@ -1227,7 +1227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F898D18F-5A5F-4E8D-A863-0FC23AACA96E}" type="CELLRANGE">
+                    <a:fld id="{0B8B3CA9-B4C5-4F80-B5CC-76E435FD96CB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1261,7 +1261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D30A8F4-9C8A-4AB8-BA48-31243B010726}" type="CELLRANGE">
+                    <a:fld id="{3CF94AAC-60B3-4AD8-8064-583CC4F0069B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1295,7 +1295,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F015EE22-4E4A-4448-8F13-7FA051F5F19F}" type="CELLRANGE">
+                    <a:fld id="{88206703-5008-4552-98F1-1875CE5B0C21}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1329,7 +1329,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2637F486-3A3B-4849-BCA3-0B150EECB720}" type="CELLRANGE">
+                    <a:fld id="{A3D5532C-5A40-4A60-8325-FFFF77C9827A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1363,7 +1363,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF9B3F25-8B00-46F2-956E-E47B80F867C2}" type="CELLRANGE">
+                    <a:fld id="{6B44DE05-1D8C-4391-B3AB-4A8EAB44322C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1560,7 +1560,7 @@
                   <c:v>37378</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39091</c:v>
+                  <c:v>40187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,7 +1624,7 @@
                     <c:v>5.58%</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>5.62%</c:v>
+                    <c:v>5.64%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1931,7 +1931,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Totals!$A$2:$A$19</c15:sqref>
@@ -2529,7 +2529,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,36 +3212,36 @@
         <v>43922</v>
       </c>
       <c r="B19" s="2">
-        <v>1713</v>
+        <v>2809</v>
       </c>
       <c r="C19" s="5">
-        <v>38371</v>
+        <v>66573</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>24762</v>
+        <v>41989</v>
       </c>
       <c r="E19" s="2">
-        <v>23049</v>
+        <v>39180</v>
       </c>
       <c r="F19" s="2">
-        <v>63133</v>
+        <v>108563</v>
       </c>
       <c r="G19" s="2">
         <f>SUM(B$2:B19)</f>
-        <v>39091</v>
+        <v>40187</v>
       </c>
       <c r="H19" s="2">
         <f>SUM(D$2:D19)</f>
-        <v>695104</v>
+        <v>712331</v>
       </c>
       <c r="I19" s="6">
         <f>G19/H19</f>
-        <v>5.6237627750667527E-2</v>
+        <v>5.6416188541562842E-2</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="5"/>
-        <v>63133</v>
+        <v>108562</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3301,15 +3301,15 @@
       </c>
       <c r="B30" s="2">
         <f>SUM(B2:B27)</f>
-        <v>39091</v>
+        <v>40187</v>
       </c>
       <c r="C30" s="2">
         <f>SUM(D2:D27)</f>
-        <v>695104</v>
+        <v>712331</v>
       </c>
       <c r="D30" s="2">
         <f>SUM(F2:F27)</f>
-        <v>1850946</v>
+        <v>1896376</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="B31" s="6">
         <f>B30/C30</f>
-        <v>5.6237627750667527E-2</v>
+        <v>5.6416188541562842E-2</v>
       </c>
       <c r="C31" s="6"/>
     </row>

</xml_diff>